<commit_message>
Changed approach to taking gems
Added a cycle in the player to call the model to predict which gem to take/discard several times.  Gets remembered after regular memory by calling player.local_memory.
</commit_message>
<xml_diff>
--- a/Splendor/Environment/Splendor_components/Board_components/Splendor_cards.xlsx
+++ b/Splendor/Environment/Splendor_components/Board_components/Splendor_cards.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Python_Files\Splendor\Environment\Splendor_components\Board_components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80636B1-946C-46F1-BD7E-AFC861C1B491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8561EDD8-0365-4224-9D29-56E1DAE1FE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19800" yWindow="2460" windowWidth="15120" windowHeight="15450" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19455" yWindow="2115" windowWidth="15120" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tier1" sheetId="1" r:id="rId1"/>
-    <sheet name="tier2" sheetId="3" r:id="rId2"/>
-    <sheet name="tier3" sheetId="4" r:id="rId3"/>
-    <sheet name="nobles" sheetId="5" r:id="rId4"/>
+    <sheet name="0" sheetId="5" r:id="rId1"/>
+    <sheet name="1" sheetId="1" r:id="rId2"/>
+    <sheet name="2" sheetId="3" r:id="rId3"/>
+    <sheet name="3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tier1!$B$1:$I$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1'!$B$1:$I$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -405,6 +405,305 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5EFF4C-5A62-4F84-A501-5E8E8E55D25C}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
@@ -1483,7 +1782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC8FF0A-6155-4E9D-B87F-19F43A26707E}">
   <dimension ref="A1:H31"/>
   <sheetViews>
@@ -2302,7 +2601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45873D6E-9ECA-41C2-9D19-942DE2FA8003}">
   <dimension ref="A1:H21"/>
   <sheetViews>
@@ -2859,305 +3158,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5EFF4C-5A62-4F84-A501-5E8E8E55D25C}">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>91</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>92</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>93</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>94</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>95</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>96</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>97</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>98</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>99</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>100</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Full multi-move gem selection
</commit_message>
<xml_diff>
--- a/Splendor/Environment/Splendor_components/Board_components/Splendor_cards.xlsx
+++ b/Splendor/Environment/Splendor_components/Board_components/Splendor_cards.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Python_Files\Splendor\Environment\Splendor_components\Board_components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80636B1-946C-46F1-BD7E-AFC861C1B491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8561EDD8-0365-4224-9D29-56E1DAE1FE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19800" yWindow="2460" windowWidth="15120" windowHeight="15450" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19455" yWindow="2115" windowWidth="15120" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tier1" sheetId="1" r:id="rId1"/>
-    <sheet name="tier2" sheetId="3" r:id="rId2"/>
-    <sheet name="tier3" sheetId="4" r:id="rId3"/>
-    <sheet name="nobles" sheetId="5" r:id="rId4"/>
+    <sheet name="0" sheetId="5" r:id="rId1"/>
+    <sheet name="1" sheetId="1" r:id="rId2"/>
+    <sheet name="2" sheetId="3" r:id="rId3"/>
+    <sheet name="3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tier1!$B$1:$I$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1'!$B$1:$I$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -405,6 +405,305 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5EFF4C-5A62-4F84-A501-5E8E8E55D25C}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
@@ -1483,7 +1782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC8FF0A-6155-4E9D-B87F-19F43A26707E}">
   <dimension ref="A1:H31"/>
   <sheetViews>
@@ -2302,7 +2601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45873D6E-9ECA-41C2-9D19-942DE2FA8003}">
   <dimension ref="A1:H21"/>
   <sheetViews>
@@ -2859,305 +3158,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5EFF4C-5A62-4F84-A501-5E8E8E55D25C}">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>91</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>92</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>93</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>94</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>95</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>96</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>97</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>98</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>99</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>100</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>